<commit_message>
relatorio de produtos por cliente
</commit_message>
<xml_diff>
--- a/Files/Kanban.xlsx
+++ b/Files/Kanban.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20414"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448C253C-9707-43C1-BFEC-30A332914CF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40DB892-DA91-4FF1-A1B3-C4818D1712CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados do Roteiro" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="65">
   <si>
     <t>Crie um Roteiro Ágil inserindo marcos ou atividades importantes na tabela Dados do Roteiro nesta planilha.
 O título desta planilha está na célula B1. 
@@ -232,6 +232,12 @@
   </si>
   <si>
     <t>Responsividade</t>
+  </si>
+  <si>
+    <t>Identificado</t>
+  </si>
+  <si>
+    <t>O Botão de voltar na home da pagina create de contas a pagar e receber ainda continua aparecendo</t>
   </si>
 </sst>
 </file>
@@ -1884,7 +1890,7 @@
   </sheetPr>
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -3819,8 +3825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C51926-15E1-421E-BB34-06A5B7F6301A}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3959,6 +3965,20 @@
       </c>
       <c r="E9" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
inicio do backend para criar o fluxo de caixa
</commit_message>
<xml_diff>
--- a/Files/Kanban.xlsx
+++ b/Files/Kanban.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20414"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40DB892-DA91-4FF1-A1B3-C4818D1712CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E401F8FE-3AB8-463E-8020-5469FB6EAA97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados do Roteiro" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="66">
   <si>
     <t>Crie um Roteiro Ágil inserindo marcos ou atividades importantes na tabela Dados do Roteiro nesta planilha.
 O título desta planilha está na célula B1. 
@@ -138,9 +138,6 @@
     <t>Documentação</t>
   </si>
   <si>
-    <t>Testes Automátizados</t>
-  </si>
-  <si>
     <t>Corrigir pendências de erros</t>
   </si>
   <si>
@@ -234,10 +231,16 @@
     <t>Responsividade</t>
   </si>
   <si>
-    <t>Identificado</t>
-  </si>
-  <si>
     <t>O Botão de voltar na home da pagina create de contas a pagar e receber ainda continua aparecendo</t>
+  </si>
+  <si>
+    <t>Desconto nas vendas</t>
+  </si>
+  <si>
+    <t>Fluxo de caixa</t>
+  </si>
+  <si>
+    <t>View de relatório de produtos por cliente</t>
   </si>
 </sst>
 </file>
@@ -1290,10 +1293,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="DadosDoRoteiro" displayName="DadosDoRoteiro" ref="B2:C32">
-  <autoFilter ref="B2:C32" xr:uid="{B80C8491-F170-48E0-963D-C66B0E84BEF8}"/>
-  <sortState ref="B3:C32">
-    <sortCondition ref="C3:C32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="DadosDoRoteiro" displayName="DadosDoRoteiro" ref="B2:C34">
+  <autoFilter ref="B2:C34" xr:uid="{B80C8491-F170-48E0-963D-C66B0E84BEF8}"/>
+  <sortState ref="B3:C34">
+    <sortCondition ref="C3:C34"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Meta" totalsRowLabel="Total"/>
@@ -1597,10 +1600,10 @@
     <tabColor theme="1" tint="0.499984740745262"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1669,7 +1672,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1778,7 +1781,7 @@
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
         <v>29</v>
@@ -1786,7 +1789,7 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C22" t="s">
         <v>31</v>
@@ -1794,7 +1797,7 @@
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
         <v>32</v>
@@ -1813,7 +1816,7 @@
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
@@ -1821,20 +1824,20 @@
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C28" t="s">
         <v>60</v>
@@ -1853,22 +1856,38 @@
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B32" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B34" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"A Fazer, Em Progresso,Concluído"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1891,7 +1910,7 @@
   <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1914,7 +1933,7 @@
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="E1" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
@@ -1943,7 +1962,7 @@
       </c>
       <c r="C3" s="12" t="str">
         <f t="array" ref="C3">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$C$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($A$3:A3)))&amp;CHAR(10),"")</f>
-        <v xml:space="preserve">View Gerar Relatório
+        <v xml:space="preserve">Otimizar Consultas
 </v>
       </c>
       <c r="D3" s="4"/>
@@ -1967,7 +1986,7 @@
       </c>
       <c r="C4" s="12" t="str">
         <f t="array" ref="C4">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$C$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($A$3:A4)))&amp;CHAR(10),"")</f>
-        <v xml:space="preserve">Testes Automátizados
+        <v xml:space="preserve">Migrar para HTTPS
 </v>
       </c>
       <c r="D4" s="4"/>
@@ -1991,13 +2010,14 @@
       </c>
       <c r="C5" s="12" t="str">
         <f t="array" ref="C5">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$C$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($A$3:A5)))&amp;CHAR(10),"")</f>
-        <v xml:space="preserve">Otimizar Consultas
+        <v xml:space="preserve">Criar método para baixar as contas ao gerar relatório mensal
 </v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="13" t="str">
         <f t="array" ref="E5">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$E$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($A$3:A5)))&amp;CHAR(10),"")</f>
-        <v/>
+        <v xml:space="preserve">Fluxo de caixa
+</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="str">
@@ -2014,7 +2034,7 @@
       </c>
       <c r="C6" s="12" t="str">
         <f t="array" ref="C6">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$C$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($A$3:A6)))&amp;CHAR(10),"")</f>
-        <v xml:space="preserve">Migrar para HTTPS
+        <v xml:space="preserve">Iteratividade nos Dashboards da Home
 </v>
       </c>
       <c r="D6" s="4"/>
@@ -2037,7 +2057,7 @@
       </c>
       <c r="C7" s="12" t="str">
         <f t="array" ref="C7">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$C$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($A$3:A7)))&amp;CHAR(10),"")</f>
-        <v xml:space="preserve">Criar método para baixar as contas ao gerar relatório mensal
+        <v xml:space="preserve">Criar Logs
 </v>
       </c>
       <c r="D7" s="4"/>
@@ -2060,7 +2080,7 @@
       </c>
       <c r="C8" s="12" t="str">
         <f t="array" ref="C8">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$C$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($A$3:A8)))&amp;CHAR(10),"")</f>
-        <v xml:space="preserve">Iteratividade nos Dashboards da Home
+        <v xml:space="preserve">Responsividade
 </v>
       </c>
       <c r="D8" s="4"/>
@@ -2083,7 +2103,7 @@
       </c>
       <c r="C9" s="12" t="str">
         <f t="array" ref="C9">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$C$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($A$3:A9)))&amp;CHAR(10),"")</f>
-        <v xml:space="preserve">Criar Logs
+        <v xml:space="preserve">Desconto nas vendas
 </v>
       </c>
       <c r="D9" s="4"/>
@@ -2106,8 +2126,7 @@
       </c>
       <c r="C10" s="12" t="str">
         <f t="array" ref="C10">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$C$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($A$3:A10)))&amp;CHAR(10),"")</f>
-        <v xml:space="preserve">Responsividade
-</v>
+        <v/>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="13" t="str">
@@ -2337,7 +2356,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4" t="str">
         <f t="array" ref="G20">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$G$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($A$3:A20)))&amp;CHAR(10),"")</f>
-        <v xml:space="preserve">Rotina de Backup
+        <v xml:space="preserve">View Gerar Relatório
 </v>
       </c>
       <c r="H20" s="4"/>
@@ -2357,7 +2376,8 @@
       </c>
       <c r="G21" s="4" t="str">
         <f t="array" ref="G21">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$G$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($A$3:A21)))&amp;CHAR(10),"")</f>
-        <v/>
+        <v xml:space="preserve">Rotina de Backup
+</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2375,7 +2395,8 @@
       </c>
       <c r="G22" s="4" t="str">
         <f t="array" ref="G22">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$G$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($A$3:A22)))&amp;CHAR(10),"")</f>
-        <v/>
+        <v xml:space="preserve">View de relatório de produtos por cliente
+</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3825,8 +3846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C51926-15E1-421E-BB34-06A5B7F6301A}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3844,7 +3865,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
@@ -3855,130 +3876,130 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
         <v>38</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
         <v>49</v>
-      </c>
-      <c r="D6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
         <v>52</v>
-      </c>
-      <c r="D7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>